<commit_message>
[Chassis] Update perimeter sketch for 2016 cup
  modified:   BaseRoulante/V2/Perimetre.xlsx

Signed-off-by: Olivier D <olivier.duval@gobgob-technology.fr>
</commit_message>
<xml_diff>
--- a/BaseRoulante/V2/Perimetre.xlsx
+++ b/BaseRoulante/V2/Perimetre.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="NonDeploye2015" sheetId="6" r:id="rId1"/>
+    <sheet name="NonDeploye2016" sheetId="4" r:id="rId2"/>
+    <sheet name="Deploye2016" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Max</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>largeur</t>
-  </si>
-  <si>
-    <t>pince</t>
   </si>
   <si>
     <t>angle</t>
@@ -42,6 +39,15 @@
     <t>roue</t>
   </si>
   <si>
+    <t>avant</t>
+  </si>
+  <si>
+    <t>LoS:</t>
+  </si>
+  <si>
+    <t>pince</t>
+  </si>
+  <si>
     <t>pince int.</t>
   </si>
 </sst>
@@ -49,6 +55,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0\°"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -107,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -127,11 +137,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -166,7 +216,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvPr id="2" name="Connecteur droit 1"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -210,7 +260,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Connecteur droit 4"/>
+        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -254,7 +304,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Connecteur droit 6"/>
+        <xdr:cNvPr id="4" name="Connecteur droit 3"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -298,7 +348,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Connecteur droit 8"/>
+        <xdr:cNvPr id="5" name="Connecteur droit 4"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -342,7 +392,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Connecteur droit 10"/>
+        <xdr:cNvPr id="6" name="Connecteur droit 5"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -386,7 +436,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Connecteur droit 12"/>
+        <xdr:cNvPr id="7" name="Connecteur droit 6"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -430,7 +480,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Connecteur droit 14"/>
+        <xdr:cNvPr id="8" name="Connecteur droit 7"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -474,7 +524,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Connecteur droit 16"/>
+        <xdr:cNvPr id="9" name="Connecteur droit 8"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -518,7 +568,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Connecteur droit avec flèche 25"/>
+        <xdr:cNvPr id="10" name="Connecteur droit avec flèche 9"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -566,7 +616,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Connecteur droit avec flèche 28"/>
+        <xdr:cNvPr id="11" name="Connecteur droit avec flèche 10"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -614,7 +664,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Connecteur droit avec flèche 30"/>
+        <xdr:cNvPr id="12" name="Connecteur droit avec flèche 11"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -662,7 +712,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Connecteur droit avec flèche 32"/>
+        <xdr:cNvPr id="13" name="Connecteur droit avec flèche 12"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -710,7 +760,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="35" name="Connecteur droit avec flèche 34"/>
+        <xdr:cNvPr id="14" name="Connecteur droit avec flèche 13"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -758,7 +808,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Connecteur droit avec flèche 36"/>
+        <xdr:cNvPr id="15" name="Connecteur droit avec flèche 14"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -806,7 +856,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="Connecteur droit avec flèche 39"/>
+        <xdr:cNvPr id="16" name="Connecteur droit avec flèche 15"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -854,7 +904,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="46" name="Connecteur droit avec flèche 45"/>
+        <xdr:cNvPr id="17" name="Connecteur droit avec flèche 16"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -902,7 +952,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="Connecteur droit avec flèche 47"/>
+        <xdr:cNvPr id="18" name="Connecteur droit avec flèche 17"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -950,7 +1000,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Connecteur droit avec flèche 50"/>
+        <xdr:cNvPr id="19" name="Connecteur droit avec flèche 18"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -975,6 +1025,2422 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Connecteur droit 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="1152525"/>
+          <a:ext cx="9525" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3810000" y="561975"/>
+          <a:ext cx="762000" cy="590551"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connecteur droit 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4562475" y="571500"/>
+          <a:ext cx="1562100" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7610476" y="4181475"/>
+          <a:ext cx="9524" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723907</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Connecteur droit 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6057907" y="4572000"/>
+          <a:ext cx="1562093" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connecteur droit 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4591051" y="4572000"/>
+          <a:ext cx="1495424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connecteur droit 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3819525" y="4000501"/>
+          <a:ext cx="762000" cy="571499"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connecteur droit avec flèche 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819525" y="581025"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connecteur droit avec flèche 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3819525" y="581025"/>
+          <a:ext cx="752476" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Connecteur droit avec flèche 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3800475" y="4695825"/>
+          <a:ext cx="2305050" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Connecteur droit avec flèche 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6115050" y="4667250"/>
+          <a:ext cx="1524000" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connecteur droit avec flèche 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6076950" y="590550"/>
+          <a:ext cx="9525" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Connecteur droit avec flèche 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2838450" y="561975"/>
+          <a:ext cx="0" cy="3971925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Connecteur droit avec flèche 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4772025" y="3438525"/>
+          <a:ext cx="9525" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connecteur droit avec flèche 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5133975" y="3505200"/>
+          <a:ext cx="495300" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connecteur droit 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6286500" y="4181475"/>
+          <a:ext cx="1343026" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connecteur droit 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6276976" y="962025"/>
+          <a:ext cx="19049" cy="3238500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connecteur droit 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7610476" y="609600"/>
+          <a:ext cx="9524" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752482</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Connecteur droit 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6086482" y="581025"/>
+          <a:ext cx="1562093" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connecteur droit 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6267450" y="971550"/>
+          <a:ext cx="1343026" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connecteur droit avec flèche 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7762875" y="4200525"/>
+          <a:ext cx="9525" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Connecteur droit 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="1152525"/>
+          <a:ext cx="9525" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3810000" y="561975"/>
+          <a:ext cx="762000" cy="590551"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connecteur droit 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4562475" y="571500"/>
+          <a:ext cx="1562100" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7610476" y="4181475"/>
+          <a:ext cx="9524" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723907</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Connecteur droit 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6057907" y="4572000"/>
+          <a:ext cx="1562093" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connecteur droit 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4591051" y="4572000"/>
+          <a:ext cx="1495424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connecteur droit 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3819525" y="4000501"/>
+          <a:ext cx="762000" cy="571499"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connecteur droit avec flèche 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819525" y="581025"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connecteur droit avec flèche 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3819525" y="581025"/>
+          <a:ext cx="752476" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Connecteur droit avec flèche 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3800475" y="4695825"/>
+          <a:ext cx="2305050" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Connecteur droit avec flèche 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6115050" y="4667250"/>
+          <a:ext cx="1524000" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connecteur droit avec flèche 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6076950" y="590550"/>
+          <a:ext cx="9525" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connecteur droit 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6286500" y="4181475"/>
+          <a:ext cx="1343026" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connecteur droit 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6276976" y="962025"/>
+          <a:ext cx="19049" cy="3238500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connecteur droit 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7610476" y="609600"/>
+          <a:ext cx="9524" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752482</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Connecteur droit 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6086482" y="581025"/>
+          <a:ext cx="1562093" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connecteur droit 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6267450" y="971550"/>
+          <a:ext cx="1343026" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594632</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>594632</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connecteur droit 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7452632" y="5905501"/>
+          <a:ext cx="762000" cy="571499"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connecteur droit avec flèche 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4562475" y="6086475"/>
+          <a:ext cx="3629025" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>617764</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>137432</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>684439</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>156482</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Connecteur droit avec flèche 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7475764" y="5852432"/>
+          <a:ext cx="828675" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>155122</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Connecteur droit avec flèche 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8537122" y="6096000"/>
+          <a:ext cx="8164" cy="408214"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>757918</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>63954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>738868</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>63954</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Connecteur droit avec flèche 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7615918" y="6540954"/>
+          <a:ext cx="742950" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Connecteur droit 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5686425" y="942975"/>
+          <a:ext cx="9525" cy="1152526"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>572860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>59874</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Connecteur droit 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7430860" y="1764847"/>
+          <a:ext cx="733425" cy="581027"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Connecteur droit avec flèche 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3829050" y="962025"/>
+          <a:ext cx="1838325" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connecteur droit avec flèche 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5695950" y="971550"/>
+          <a:ext cx="2400300" cy="729343"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Connecteur droit avec flèche 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191499" y="1755321"/>
+          <a:ext cx="0" cy="4708072"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Connecteur droit avec flèche 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4577443" y="2149929"/>
+          <a:ext cx="1110343" cy="27214"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>440872</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Connecteur droit avec flèche 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5774872" y="2190750"/>
+          <a:ext cx="1845128" cy="40821"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>536123</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>557894</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Connecteur droit avec flèche 46"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7394123" y="5878285"/>
+          <a:ext cx="21771" cy="258536"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>522516</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Connecteur droit avec flèche 51"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7380516" y="5769429"/>
+          <a:ext cx="253091" cy="27214"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1273,7 +3739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -1318,7 +3784,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>50</v>
@@ -1473,7 +3939,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J11" s="2">
         <v>152</v>
@@ -1495,7 +3961,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1526,7 +3992,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1564,7 +4030,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
@@ -1641,7 +4107,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H19" s="5">
         <f>70+10</f>
@@ -1774,7 +4240,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" s="2">
         <v>200</v>
@@ -1852,24 +4318,1151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2">
+        <f>F3</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="3">
+        <f>SQRT(E4^2+F3^2)</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="6">
+        <f>400-50</f>
+        <v>350</v>
+      </c>
+      <c r="E13" s="1">
+        <f>H16-2*E4</f>
+        <v>250</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="4">
+        <f>E13+2*F5+2*G24+2*I26+H16</f>
+        <v>1191.4213562373095</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
+        <f>1200-20</f>
+        <v>1180</v>
+      </c>
+      <c r="H16" s="2">
+        <v>350</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="5">
+        <f>70+10</f>
+        <v>80</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5">
+        <f>60+30</f>
+        <v>90</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1">
+        <v>20</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <f>H26-F3</f>
+        <v>150</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="2">
+        <v>200</v>
+      </c>
+      <c r="I26" s="2">
+        <v>75</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>$G$16</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A6:O37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="1:15">
+      <c r="J6" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="J7" s="11">
+        <f>SQRT((H9-L10)^2+(I11+K12)^2)</f>
+        <v>215.84310682341766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="G8" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="9">
+        <f>SQRT((G11+F11)^2+(H9+E12)^2)</f>
+        <v>305.16389039334257</v>
+      </c>
+      <c r="H9" s="8">
+        <v>200</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="9">
+        <f>L33</f>
+        <v>21.819805153394636</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <f>NonDeploye2016!F3</f>
+        <v>50</v>
+      </c>
+      <c r="G11" s="1">
+        <v>125</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <f>H34-F11-G11+I34</f>
+        <v>100</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2">
+        <f>F11</f>
+        <v>50</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="9">
+        <f>K36</f>
+        <v>21.81980515339464</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="3">
+        <f>SQRT(E12^2+F11^2)</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="E21" s="1">
+        <f>H24-2*E12</f>
+        <v>250</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="4">
+        <f>E21+F31+J35+L24+J7+G9</f>
+        <v>1483.1396904107669</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <f>1500-20</f>
+        <v>1480</v>
+      </c>
+      <c r="H24" s="2">
+        <f>NonDeploye2016!H16</f>
+        <v>350</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="9">
+        <f>H24+L33+L10</f>
+        <v>393.63961030678922</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3">
+        <f>F13</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1">
+        <v>10</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
+        <f>H34-F11</f>
+        <v>150</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1">
+        <v>10</v>
+      </c>
+      <c r="K32" s="12">
+        <v>45</v>
+      </c>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="2">
+        <v>45</v>
+      </c>
+      <c r="L33" s="9">
+        <f>K33*SIN(RADIANS(K32))-J32</f>
+        <v>21.819805153394636</v>
+      </c>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="2">
+        <f>NonDeploye2016!H26</f>
+        <v>200</v>
+      </c>
+      <c r="I34" s="2">
+        <f>NonDeploye2016!I26</f>
+        <v>75</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="9">
+        <f>SQRT((G32+I34+K36)^2+L33^2)</f>
+        <v>247.78240476856263</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="9">
+        <f>K33*COS(RADIANS(K32))-J31</f>
+        <v>21.81980515339464</v>
+      </c>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>$G$24</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>